<commit_message>
Calculation of enzyme kinematic parameters
Using the Lineweaver-Burk, Eadie-Hofstee or the Hanes-Woolf (a bonus) representations.
</commit_message>
<xml_diff>
--- a/DecompositionPeroxyde.xlsx
+++ b/DecompositionPeroxyde.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrener/Projects/Repzilon.Libraries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E2C3E67B-F128-7841-A10B-1EC743274A64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A10AADA-B4D7-7449-AADA-A311F7481E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7960" yWindow="3820" windowWidth="28040" windowHeight="17440" xr2:uid="{B01D318F-86D7-4149-9556-C9473594BE32}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14400" activeTab="1" xr2:uid="{B01D318F-86D7-4149-9556-C9473594BE32}"/>
   </bookViews>
   <sheets>
     <sheet name="Gráfico1" sheetId="2" r:id="rId1"/>
     <sheet name="Hoja1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,12 +37,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>s</t>
   </si>
   <si>
     <t>v</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>2*</t>
   </si>
 </sst>
 </file>
@@ -1175,7 +1184,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{94321E56-0937-BF4A-A850-6577C2018145}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="124" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="94" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1186,7 +1195,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8674919" cy="6288548"/>
+    <xdr:ext cx="8673830" cy="6282447"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1">
@@ -1512,10 +1521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B5621EF-2F33-5D4E-AA64-015F90897498}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:B6"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1524,31 +1533,54 @@
     <col min="2" max="2" width="6.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>12.5</v>
       </c>
       <c r="B2">
         <v>3.6999999999999998E-2</v>
       </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>5.9481399999999997E-2</v>
+      </c>
+      <c r="F2">
+        <f>2*E2</f>
+        <v>0.11896279999999999</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>20</v>
       </c>
       <c r="B3" s="1">
         <v>0.05</v>
       </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>-2.7960800000000001E-2</v>
+      </c>
+      <c r="F3">
+        <f>2*E3</f>
+        <v>-5.5921600000000002E-2</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>25</v>
       </c>
@@ -1556,7 +1588,7 @@
         <v>5.5E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>50</v>
       </c>
@@ -1564,7 +1596,7 @@
         <v>7.2999999999999995E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>100</v>
       </c>

</xml_diff>

<commit_message>
Recompressed an Excel spreadsheet
</commit_message>
<xml_diff>
--- a/DecompositionPeroxyde.xlsx
+++ b/DecompositionPeroxyde.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrener/Projects/Repzilon.Libraries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A10AADA-B4D7-7449-AADA-A311F7481E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C665D938-4E03-114C-A07A-7851D92A138C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14400" activeTab="1" xr2:uid="{B01D318F-86D7-4149-9556-C9473594BE32}"/>
+    <workbookView xWindow="25600" yWindow="-7500" windowWidth="38400" windowHeight="23500" activeTab="3" xr2:uid="{B01D318F-86D7-4149-9556-C9473594BE32}"/>
   </bookViews>
   <sheets>
-    <sheet name="Gráfico1" sheetId="2" r:id="rId1"/>
-    <sheet name="Hoja1" sheetId="1" r:id="rId2"/>
+    <sheet name="Michaelis-Menten lin." sheetId="2" r:id="rId1"/>
+    <sheet name="Michaelis-Menten log." sheetId="4" r:id="rId2"/>
+    <sheet name="Linéaire direct" sheetId="5" r:id="rId3"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,12 +39,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>s</t>
-  </si>
-  <si>
-    <t>v</t>
   </si>
   <si>
     <t>a</t>
@@ -51,7 +50,86 @@
     <t>b</t>
   </si>
   <si>
-    <t>2*</t>
+    <t>Modèle</t>
+  </si>
+  <si>
+    <r>
+      <t>v</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Corps)"/>
+      </rPr>
+      <t>max</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>k</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Corps)"/>
+      </rPr>
+      <t>m</t>
+    </r>
+  </si>
+  <si>
+    <t>Paramètre</t>
+  </si>
+  <si>
+    <t>Valeur</t>
+  </si>
+  <si>
+    <t>Hanes-Woolf</t>
+  </si>
+  <si>
+    <t>Observée</t>
+  </si>
+  <si>
+    <t>Modélisée</t>
+  </si>
+  <si>
+    <t>Régressée</t>
+  </si>
+  <si>
+    <t>Logarithmique</t>
+  </si>
+  <si>
+    <r>
+      <t>log</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Corps)"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(s)</t>
+    </r>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -61,13 +139,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Corps)"/>
     </font>
   </fonts>
   <fills count="2">
@@ -90,15 +174,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF3E3C54"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -113,7 +208,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-MX"/>
+  <c:lang val="fr-CA"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -131,12 +226,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -144,14 +236,9 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="es-MX"/>
-              <a:t>Vitesse</a:t>
+              <a:rPr lang="es-MX" b="1"/>
+              <a:t>Vitesse de décomposition du peroxyde</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="es-MX" baseline="0"/>
-              <a:t> de décomposition du peroxyde</a:t>
-            </a:r>
-            <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -168,19 +255,16 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CA"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -195,11 +279,198 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$B$1</c:f>
+              <c:f>Hoja1!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>v</c:v>
+                  <c:v>Observée</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$A$2:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$C$2:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>3.6999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>5.5E-2</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>7.2999999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>9.0999999999999998E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-ABE7-9D4E-BA24-20E373791F2E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Régressée</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$A$2:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$D$2:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3.7284943247737408E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.9426285584087536E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.5190628831824941E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.3096314415912467E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.1002E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0F55-8142-B8CA-CF52223F4A35}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Modélisée</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -228,6 +499,483 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$A$2:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$E$2:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3.6519358125318382E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.9059024807527794E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.5399922720247283E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.4713392391870748E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.0485957715367618E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-0F55-8142-B8CA-CF52223F4A35}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1022985935"/>
+        <c:axId val="1022814975"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1022985935"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX" sz="1200" b="1"/>
+                  <a:t>Concentration de peroxyde (mmol/L)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1022814975"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:minorUnit val="2"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1022814975"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.03"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX" sz="1200" b="1"/>
+                  <a:t>Vitesse</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0.000" sourceLinked="0"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1022985935"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="tr"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.83066061935730817"/>
+          <c:y val="0.74409589129840636"/>
+          <c:w val="0.13892847796186922"/>
+          <c:h val="0.13645256378605344"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1440" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-CA" b="1"/>
+              <a:t>Vitesse de décomposition du peroxyde</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1440" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Observée</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
           <c:trendline>
             <c:spPr>
               <a:ln w="19050" cap="rnd">
@@ -238,7 +986,8 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="log"/>
+            <c:trendlineType val="linear"/>
+            <c:backward val="0.6"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -255,50 +1004,47 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
+                        <a:schemeClr val="tx1"/>
                       </a:solidFill>
                       <a:latin typeface="+mn-lt"/>
                       <a:ea typeface="+mn-ea"/>
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="es-CA"/>
+                  <a:endParaRPr lang="fr-FR"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja1!$A$2:$A$6</c:f>
+              <c:f>Hoja1!$B$2:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>12.5</c:v>
+                  <c:v>1.0969100130080565</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>1.3010299956639813</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25</c:v>
+                  <c:v>1.3979400086720377</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>50</c:v>
+                  <c:v>1.6989700043360187</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$B$2:$B$6</c:f>
+              <c:f>Hoja1!$C$2:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
@@ -323,7 +1069,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-ABE7-9D4E-BA24-20E373791F2E}"/>
+              <c16:uniqueId val="{00000000-179C-A94C-BBD3-1B40A2C9579E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -335,11 +1081,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1022985935"/>
-        <c:axId val="1022814975"/>
+        <c:axId val="682783248"/>
+        <c:axId val="683375952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1022985935"/>
+        <c:axId val="682783248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -366,12 +1112,9 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -379,14 +1122,9 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="es-MX"/>
-                  <a:t>Concentration de peroxyde</a:t>
+                  <a:rPr lang="fr-CA" b="1"/>
+                  <a:t>Logarithme en base 10 de la concentration de peroxyde (mmol/L)</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="es-MX" baseline="0"/>
-                  <a:t> (mmol/L)</a:t>
-                </a:r>
-                <a:endParaRPr lang="es-MX"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -403,34 +1141,28 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CA"/>
+              <a:endParaRPr lang="fr-FR"/>
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -441,27 +1173,24 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CA"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1022814975"/>
+        <c:crossAx val="683375952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1022814975"/>
+        <c:axId val="683375952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -488,12 +1217,9 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -501,7 +1227,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="es-MX"/>
+                  <a:rPr lang="fr-CA"/>
                   <a:t>Vitesse</a:t>
                 </a:r>
               </a:p>
@@ -520,34 +1246,28 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CA"/>
+              <a:endParaRPr lang="fr-FR"/>
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
+        <c:numFmt formatCode="#,##0.000" sourceLinked="0"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -558,29 +1278,30 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CA"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1022985935"/>
+        <c:crossAx val="682783248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.02"/>
+        <c:minorUnit val="5.0000000000000001E-3"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
-          <a:noFill/>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
@@ -616,9 +1337,762 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr sz="1200">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="es-CA"/>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-CA" b="1"/>
+              <a:t>Vitesse de décomposition du peroxyde</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>12,5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="35"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$K$3:$K$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>-12.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$L$3:$L$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.6999999999999998E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-40F9-E64C-8438-F08CF3D13CB2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="35"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$M$3:$M$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$N$3:$N$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-40F9-E64C-8438-F08CF3D13CB2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$O$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="35"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$O$3:$O$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>-25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$P$3:$P$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.5E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-40F9-E64C-8438-F08CF3D13CB2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$Q$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="35"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$Q$3:$Q$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>-50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$R$3:$R$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.2999999999999995E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-40F9-E64C-8438-F08CF3D13CB2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$S$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="35"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$S$3:$S$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>-100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$T$3:$T$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.0999999999999998E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-40F9-E64C-8438-F08CF3D13CB2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="477823376"/>
+        <c:axId val="575689376"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="477823376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="40"/>
+          <c:min val="-100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-CA" sz="1200" b="1"/>
+                  <a:t>Concentration en</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-CA" sz="1200" b="1" baseline="0"/>
+                  <a:t> peroxyde (mmol/L)</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-CA" sz="1200" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="575689376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="575689376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.14000000000000001"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-CA" sz="1200" b="1"/>
+                  <a:t>Vitesse</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0.000" sourceLinked="0"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="477823376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -664,6 +2138,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1180,11 +2734,1065 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{94321E56-0937-BF4A-A850-6577C2018145}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="94" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="202" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{3C8045FA-2993-9C48-9764-04C23805502A}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="184" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{F035F398-36C9-8943-B3D5-681A60E7C6CD}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="184" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1195,7 +3803,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8673830" cy="6282447"/>
+    <xdr:ext cx="8672286" cy="6284686"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1">
@@ -1224,10 +3832,76 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8672286" cy="6284686"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8BC4474-3ACB-6C3F-92E4-26011A7DC373}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8676033" cy="6287880"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96EAF1A4-829F-D4B9-4CBF-896EBB1E1AF8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1265,7 +3939,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1371,7 +4045,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1513,7 +4187,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1521,90 +4195,325 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B5621EF-2F33-5D4E-AA64-015F90897498}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="3">
+        <f>A2</f>
+        <v>12.5</v>
+      </c>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3">
+        <f>A3</f>
+        <v>20</v>
+      </c>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3">
+        <f>A4</f>
+        <v>25</v>
+      </c>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3">
+        <f>A5</f>
+        <v>50</v>
+      </c>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3">
+        <f>A6</f>
+        <v>100</v>
+      </c>
+      <c r="T1" s="3"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>12.5</v>
       </c>
       <c r="B2">
+        <f>LOG10(A2)</f>
+        <v>1.0969100130080565</v>
+      </c>
+      <c r="C2">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="D2" t="s">
-        <v>2</v>
+      <c r="D2">
+        <f>$I$2*LOG10(A2)+$I$3</f>
+        <v>3.7284943247737408E-2</v>
       </c>
       <c r="E2">
+        <f>($I$4*A2)/($I$5+A2)</f>
+        <v>3.6519358125318382E-2</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2">
         <v>5.9481399999999997E-2</v>
       </c>
-      <c r="F2">
-        <f>2*E2</f>
-        <v>0.11896279999999999</v>
+      <c r="K2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>14</v>
+      </c>
+      <c r="R2" t="s">
+        <v>15</v>
+      </c>
+      <c r="S2" t="s">
+        <v>14</v>
+      </c>
+      <c r="T2" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>20</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3">
+        <f t="shared" ref="B3:B6" si="0">LOG10(A3)</f>
+        <v>1.3010299956639813</v>
+      </c>
+      <c r="C3" s="1">
         <v>0.05</v>
       </c>
-      <c r="D3" t="s">
-        <v>3</v>
+      <c r="D3">
+        <f t="shared" ref="D3:D6" si="1">$I$2*LOG10(A3)+$I$3</f>
+        <v>4.9426285584087536E-2</v>
       </c>
       <c r="E3">
+        <f t="shared" ref="E3:E6" si="2">($I$4*A3)/($I$5+A3)</f>
+        <v>4.9059024807527794E-2</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3">
         <v>-2.7960800000000001E-2</v>
       </c>
-      <c r="F3">
-        <f>2*E3</f>
-        <v>-5.5921600000000002E-2</v>
+      <c r="K3">
+        <f>-1*K1</f>
+        <v>-12.5</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <f>-1*M1</f>
+        <v>-20</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <f>-1*O1</f>
+        <v>-25</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <f>-1*Q1</f>
+        <v>-50</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <f>-1*S1</f>
+        <v>-100</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>25</v>
       </c>
       <c r="B4">
+        <f t="shared" si="0"/>
+        <v>1.3979400086720377</v>
+      </c>
+      <c r="C4">
         <v>5.5E-2</v>
       </c>
+      <c r="D4">
+        <f t="shared" si="1"/>
+        <v>5.5190628831824941E-2</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="2"/>
+        <v>5.5399922720247283E-2</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4">
+        <v>0.1147</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <f>C2</f>
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4" s="1">
+        <f>C3</f>
+        <v>0.05</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <f>C4</f>
+        <v>5.5E-2</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <f>C5</f>
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <f>C6</f>
+        <v>9.0999999999999998E-2</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>50</v>
       </c>
       <c r="B5">
+        <f t="shared" si="0"/>
+        <v>1.6989700043360187</v>
+      </c>
+      <c r="C5">
         <v>7.2999999999999995E-2</v>
       </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>7.3096314415912467E-2</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="2"/>
+        <v>7.4713392391870748E-2</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5">
+        <v>26.76</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>100</v>
       </c>
       <c r="B6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C6">
         <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>9.1002E-2</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="2"/>
+        <v>9.0485957715367618E-2</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Trying out the Michaelis-Menten cheat code
</commit_message>
<xml_diff>
--- a/DecompositionPeroxyde.xlsx
+++ b/DecompositionPeroxyde.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrener/Projects/Repzilon.Libraries/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Administrator\source\repos\repzilon\Repzilon.Libraries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C665D938-4E03-114C-A07A-7851D92A138C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{677927C8-2C2B-4558-9815-4CC7C30BCAE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="-7500" windowWidth="38400" windowHeight="23500" activeTab="3" xr2:uid="{B01D318F-86D7-4149-9556-C9473594BE32}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{B01D318F-86D7-4149-9556-C9473594BE32}"/>
   </bookViews>
   <sheets>
     <sheet name="Michaelis-Menten lin." sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>s</t>
   </si>
@@ -87,9 +87,6 @@
     <t>Valeur</t>
   </si>
   <si>
-    <t>Hanes-Woolf</t>
-  </si>
-  <si>
     <t>Observée</t>
   </si>
   <si>
@@ -131,15 +128,31 @@
   <si>
     <t>y</t>
   </si>
+  <si>
+    <t>Graphique linéaire direct</t>
+  </si>
+  <si>
+    <t>(0; v)</t>
+  </si>
+  <si>
+    <t>(-s; 0)</t>
+  </si>
+  <si>
+    <t>Axes</t>
+  </si>
+  <si>
+    <t>Michaelis-Menten</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -174,15 +187,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -208,7 +223,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="fr-CA"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -530,19 +545,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>3.6519358125318382E-2</c:v>
+                  <c:v>3.7645116017564408E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.9059024807527794E-2</c:v>
+                  <c:v>4.9427685469272516E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.5399922720247283E-2</c:v>
+                  <c:v>5.5185165836432855E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.4713392391870748E-2</c:v>
+                  <c:v>7.1946161575092357E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.0485957715367618E-2</c:v>
+                  <c:v>8.482830944569146E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -872,7 +887,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="fr-CA"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1227,7 +1242,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="fr-CA"/>
+                  <a:rPr lang="fr-CA" b="1"/>
                   <a:t>Vitesse</a:t>
                 </a:r>
               </a:p>
@@ -1352,7 +1367,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="fr-CA"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1423,7 +1438,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$K$1</c:f>
+              <c:f>Hoja1!$L$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1461,7 +1476,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja1!$K$3:$K$4</c:f>
+              <c:f>Hoja1!$L$4:$L$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1476,7 +1491,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$L$3:$L$4</c:f>
+              <c:f>Hoja1!$M$4:$M$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1501,7 +1516,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$M$1</c:f>
+              <c:f>Hoja1!$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1539,7 +1554,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja1!$M$3:$M$4</c:f>
+              <c:f>Hoja1!$N$4:$N$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1554,7 +1569,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$N$3:$N$4</c:f>
+              <c:f>Hoja1!$O$4:$O$5</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1579,7 +1594,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$O$1</c:f>
+              <c:f>Hoja1!$P$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1617,7 +1632,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja1!$O$3:$O$4</c:f>
+              <c:f>Hoja1!$P$4:$P$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1632,7 +1647,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$P$3:$P$4</c:f>
+              <c:f>Hoja1!$Q$4:$Q$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1657,7 +1672,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$Q$1</c:f>
+              <c:f>Hoja1!$R$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1699,7 +1714,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja1!$Q$3:$Q$4</c:f>
+              <c:f>Hoja1!$R$4:$R$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1714,7 +1729,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$R$3:$R$4</c:f>
+              <c:f>Hoja1!$S$4:$S$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1739,7 +1754,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$S$1</c:f>
+              <c:f>Hoja1!$T$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1781,7 +1796,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja1!$S$3:$S$4</c:f>
+              <c:f>Hoja1!$T$4:$T$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1796,7 +1811,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$T$3:$T$4</c:f>
+              <c:f>Hoja1!$U$4:$U$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -3770,7 +3785,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{94321E56-0937-BF4A-A850-6577C2018145}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="202" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="132" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3781,7 +3796,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{3C8045FA-2993-9C48-9764-04C23805502A}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="184" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="132" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3792,7 +3807,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{F035F398-36C9-8943-B3D5-681A60E7C6CD}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="184" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="132" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3803,7 +3818,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8672286" cy="6284686"/>
+    <xdr:ext cx="8672180" cy="6302006"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1">
@@ -3836,7 +3851,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8672286" cy="6284686"/>
+    <xdr:ext cx="8659091" cy="6285057"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Graphique 1">
@@ -3869,7 +3884,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8676033" cy="6287880"/>
+    <xdr:ext cx="8659091" cy="6285057"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Graphique 1">
@@ -4195,47 +4210,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B5621EF-2F33-5D4E-AA64-015F90897498}">
-  <dimension ref="A1:T6"/>
+  <dimension ref="A1:U6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="3.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="3.83203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="4.83203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="19.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
         <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
@@ -4246,33 +4262,20 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="3">
-        <f>A2</f>
-        <v>12.5</v>
-      </c>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3">
-        <f>A3</f>
-        <v>20</v>
-      </c>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3">
-        <f>A4</f>
-        <v>25</v>
-      </c>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3">
-        <f>A5</f>
-        <v>50</v>
-      </c>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3">
-        <f>A6</f>
-        <v>100</v>
-      </c>
-      <c r="T1" s="3"/>
+      <c r="L1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21">
       <c r="A2">
         <v>12.5</v>
       </c>
@@ -4289,10 +4292,10 @@
       </c>
       <c r="E2">
         <f>($I$4*A2)/($I$5+A2)</f>
-        <v>3.6519358125318382E-2</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>12</v>
+        <v>3.7645116017564408E-2</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="H2" t="s">
         <v>1</v>
@@ -4301,37 +4304,35 @@
         <v>5.9481399999999997E-2</v>
       </c>
       <c r="K2" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" t="s">
-        <v>15</v>
-      </c>
-      <c r="M2" t="s">
-        <v>14</v>
-      </c>
-      <c r="N2" t="s">
-        <v>15</v>
-      </c>
-      <c r="O2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P2" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>14</v>
-      </c>
-      <c r="R2" t="s">
-        <v>15</v>
-      </c>
-      <c r="S2" t="s">
-        <v>14</v>
-      </c>
-      <c r="T2" t="s">
-        <v>15</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="L2" s="2">
+        <f>A2</f>
+        <v>12.5</v>
+      </c>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2">
+        <f>A3</f>
+        <v>20</v>
+      </c>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2">
+        <f>A4</f>
+        <v>25</v>
+      </c>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2">
+        <f>A5</f>
+        <v>50</v>
+      </c>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2">
+        <f>A6</f>
+        <v>100</v>
+      </c>
+      <c r="U2" s="2"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21">
       <c r="A3">
         <v>20</v>
       </c>
@@ -4348,52 +4349,50 @@
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E6" si="2">($I$4*A3)/($I$5+A3)</f>
-        <v>4.9059024807527794E-2</v>
-      </c>
-      <c r="G3" s="2"/>
+        <v>4.9427685469272516E-2</v>
+      </c>
+      <c r="G3" s="3"/>
       <c r="H3" t="s">
         <v>2</v>
       </c>
       <c r="I3">
         <v>-2.7960800000000001E-2</v>
       </c>
-      <c r="K3">
-        <f>-1*K1</f>
-        <v>-12.5</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <f>-1*M1</f>
-        <v>-20</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <f>-1*O1</f>
-        <v>-25</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <f>-1*Q1</f>
-        <v>-50</v>
-      </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <f>-1*S1</f>
-        <v>-100</v>
-      </c>
-      <c r="T3">
-        <v>0</v>
+      <c r="K3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M3" t="s">
+        <v>14</v>
+      </c>
+      <c r="N3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>14</v>
+      </c>
+      <c r="R3" t="s">
+        <v>13</v>
+      </c>
+      <c r="S3" t="s">
+        <v>14</v>
+      </c>
+      <c r="T3" t="s">
+        <v>13</v>
+      </c>
+      <c r="U3" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="19.5">
       <c r="A4">
         <v>25</v>
       </c>
@@ -4410,54 +4409,58 @@
       </c>
       <c r="E4">
         <f t="shared" si="2"/>
-        <v>5.5399922720247283E-2</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>8</v>
+        <v>5.5185165836432855E-2</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="H4" t="s">
         <v>4</v>
       </c>
-      <c r="I4">
-        <v>0.1147</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
+      <c r="I4" s="4">
+        <f>I2*4/LN(10)</f>
+        <v>0.10332977518352032</v>
+      </c>
+      <c r="K4" t="s">
+        <v>17</v>
       </c>
       <c r="L4">
-        <f>C2</f>
-        <v>3.6999999999999998E-2</v>
+        <f>-1*L2</f>
+        <v>-12.5</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
-      <c r="N4" s="1">
-        <f>C3</f>
-        <v>0.05</v>
+      <c r="N4">
+        <f>-1*N2</f>
+        <v>-20</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4">
-        <f>C4</f>
-        <v>5.5E-2</v>
+        <f>-1*P2</f>
+        <v>-25</v>
       </c>
       <c r="Q4">
         <v>0</v>
       </c>
       <c r="R4">
-        <f>C5</f>
-        <v>7.2999999999999995E-2</v>
+        <f>-1*R2</f>
+        <v>-50</v>
       </c>
       <c r="S4">
         <v>0</v>
       </c>
       <c r="T4">
-        <f>C6</f>
-        <v>9.0999999999999998E-2</v>
+        <f>-1*T2</f>
+        <v>-100</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="19.5">
       <c r="A5">
         <v>50</v>
       </c>
@@ -4474,17 +4477,56 @@
       </c>
       <c r="E5">
         <f t="shared" si="2"/>
-        <v>7.4713392391870748E-2</v>
-      </c>
-      <c r="G5" s="2"/>
+        <v>7.1946161575092357E-2</v>
+      </c>
+      <c r="G5" s="3"/>
       <c r="H5" t="s">
         <v>5</v>
       </c>
-      <c r="I5">
-        <v>26.76</v>
+      <c r="I5" s="5">
+        <f>10^((0.5*I4-I3)/I2)</f>
+        <v>21.810485035863902</v>
+      </c>
+      <c r="K5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <f>C2</f>
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5" s="1">
+        <f>C3</f>
+        <v>0.05</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <f>C4</f>
+        <v>5.5E-2</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <f>C5</f>
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <f>C6</f>
+        <v>9.0999999999999998E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21">
       <c r="A6">
         <v>100</v>
       </c>
@@ -4501,18 +4543,19 @@
       </c>
       <c r="E6">
         <f t="shared" si="2"/>
-        <v>9.0485957715367618E-2</v>
+        <v>8.482830944569146E-2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="S1:T1"/>
+  <mergeCells count="8">
+    <mergeCell ref="L1:U1"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="T2:U2"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="G4:G5"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="P2:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>